<commit_message>
Relatório Final p/ Entrega 1
</commit_message>
<xml_diff>
--- a/PA/Cronograma_Projeto.xlsx
+++ b/PA/Cronograma_Projeto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive - Instituto Politécnico do Cávado e do Ave\Ambiente de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd9d8dc938d9c9fa/Universidade/3_Ano/1_Semestre/SMARTCAMPUS/PA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5E5376E-A2A1-456D-91C2-BC77CF29F993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{A5E5376E-A2A1-456D-91C2-BC77CF29F993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AA9CEB4-7954-4BE6-BC73-ABBBC31FDEDE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="3" r:id="rId1"/>
@@ -382,14 +382,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -398,6 +390,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,13 +732,13 @@
     <col min="6" max="6" width="4.140625" customWidth="1"/>
     <col min="7" max="7" width="33.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.140625" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="4.140625" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="4.140625" customWidth="1"/>
     <col min="13" max="13" width="32.7109375" customWidth="1"/>
     <col min="14" max="14" width="4.140625" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1"/>
     <col min="16" max="16" width="4.140625" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
@@ -779,38 +779,38 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="32" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="32" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="32" t="s">
+      <c r="K3" s="39"/>
+      <c r="L3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="M3" s="39"/>
+      <c r="N3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="32" t="s">
+      <c r="O3" s="39"/>
+      <c r="P3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="33"/>
+      <c r="Q3" s="39"/>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="9">
@@ -847,8 +847,8 @@
     </row>
     <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36">
+      <c r="B5" s="37"/>
+      <c r="C5" s="32">
         <v>2</v>
       </c>
       <c r="D5" s="10">
@@ -858,7 +858,7 @@
       <c r="F5" s="10">
         <v>26</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="34" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="10">
@@ -886,7 +886,7 @@
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="9">
@@ -925,7 +925,7 @@
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="35"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="9">
         <v>4</v>
       </c>
@@ -962,7 +962,7 @@
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="35"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="9">
         <v>5</v>
       </c>
@@ -973,7 +973,7 @@
       <c r="F8" s="10">
         <v>17</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="33" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="10">
@@ -1001,7 +1001,7 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="35"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="9">
         <v>6</v>
       </c>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="9">
@@ -1072,7 +1072,7 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="35"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="9">
         <v>8</v>
       </c>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="35"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="9">
         <v>9</v>
       </c>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="35"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="9">
         <v>10</v>
       </c>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="9">
@@ -1212,7 +1212,7 @@
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="35"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="9">
         <v>12</v>
       </c>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="35"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="9">
         <v>13</v>
       </c>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="35"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="9">
         <v>14</v>
       </c>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="35"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="9">
         <v>15</v>
       </c>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="36" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="9">
@@ -1387,7 +1387,7 @@
     </row>
     <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="35"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="9">
         <v>17</v>
       </c>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="35"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="9">
         <v>18</v>
       </c>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="35"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="9">
         <v>19</v>
       </c>
@@ -1505,7 +1505,7 @@
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="23"/>
       <c r="F25" s="28"/>
-      <c r="G25" s="39"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
@@ -6077,11 +6077,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="F3:G3"/>
@@ -6089,6 +6084,11 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
PA: Entrega 3 Concluída.
</commit_message>
<xml_diff>
--- a/PA/Cronograma_Projeto.xlsx
+++ b/PA/Cronograma_Projeto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive - Instituto Politécnico do Cávado e do Ave\Ambiente de Trabalho\LESI3_SmartCampus\PA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Documents\SmartEnergy\PA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2066B4-D751-44C7-AA03-2046DAA10757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271B2744-1A2B-41F4-A376-BCA4D9733CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="3" r:id="rId1"/>
@@ -98,13 +98,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Primeira Entrega</t>
-  </si>
-  <si>
     <t>Reunião final</t>
-  </si>
-  <si>
-    <t>Segunda Entrega</t>
   </si>
   <si>
     <t>Reunião(Definição dos casos de uso)</t>
@@ -131,9 +125,6 @@
     <t>Reunião(Validação das atas e convocatórias)</t>
   </si>
   <si>
-    <t>Terceira entrega</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Reunião (Realização do diagrama de estados)</t>
   </si>
   <si>
@@ -150,6 +141,15 @@
   </si>
   <si>
     <t>Reunião final(Revisão geral)</t>
+  </si>
+  <si>
+    <t>1ª Entrega</t>
+  </si>
+  <si>
+    <t>2ª Entrega</t>
+  </si>
+  <si>
+    <t>3ª entrega</t>
   </si>
 </sst>
 </file>
@@ -499,14 +499,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -527,6 +519,14 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,8 +847,8 @@
   </sheetPr>
   <dimension ref="A1:Q924"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="117" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="174" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -856,20 +856,18 @@
     <col min="1" max="1" width="0.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.140625" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="4" max="6" width="4.140625" customWidth="1"/>
     <col min="7" max="7" width="40.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
     <col min="10" max="10" width="4.140625" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
     <col min="12" max="12" width="4.140625" customWidth="1"/>
     <col min="13" max="13" width="48.7109375" customWidth="1"/>
     <col min="14" max="14" width="4.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
     <col min="16" max="16" width="4.140625" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -908,38 +906,38 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="37" t="s">
+      <c r="E3" s="52"/>
+      <c r="F3" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="52"/>
+      <c r="H3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="37" t="s">
+      <c r="I3" s="52"/>
+      <c r="J3" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="52"/>
+      <c r="L3" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="37" t="s">
+      <c r="M3" s="52"/>
+      <c r="N3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="37" t="s">
+      <c r="O3" s="52"/>
+      <c r="P3" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="38"/>
+      <c r="Q3" s="52"/>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="53" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="9">
@@ -976,7 +974,7 @@
     </row>
     <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="36"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="9">
         <v>2</v>
       </c>
@@ -1015,7 +1013,7 @@
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="53" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="9">
@@ -1054,7 +1052,7 @@
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="36"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="9">
         <v>4</v>
       </c>
@@ -1091,7 +1089,7 @@
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="36"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="9">
         <v>5</v>
       </c>
@@ -1103,7 +1101,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="10">
         <v>18</v>
@@ -1121,7 +1119,7 @@
         <v>21</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="P8" s="10">
         <v>22</v>
@@ -1130,7 +1128,7 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="36"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="9">
         <v>6</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>24</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H9" s="10">
         <v>25</v>
@@ -1156,7 +1154,7 @@
         <v>27</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N9" s="10">
         <v>28</v>
@@ -1169,7 +1167,7 @@
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="53" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="9">
@@ -1183,7 +1181,7 @@
         <v>31</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10" s="10">
         <v>1</v>
@@ -1197,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N10" s="10">
         <v>4</v>
@@ -1210,7 +1208,7 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="36"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="9">
         <v>8</v>
       </c>
@@ -1222,7 +1220,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H11" s="10">
         <v>8</v>
@@ -1236,7 +1234,7 @@
         <v>10</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N11" s="10">
         <v>11</v>
@@ -1249,7 +1247,7 @@
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="36"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="9">
         <v>9</v>
       </c>
@@ -1261,7 +1259,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H12" s="10">
         <v>15</v>
@@ -1274,13 +1272,13 @@
         <v>17</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N12" s="10">
         <v>18</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="P12" s="10">
         <v>19</v>
@@ -1289,7 +1287,7 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="36"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="9">
         <v>10</v>
       </c>
@@ -1301,7 +1299,7 @@
         <v>21</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H13" s="10">
         <v>22</v>
@@ -1315,7 +1313,7 @@
         <v>24</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N13" s="10">
         <v>25</v>
@@ -1328,7 +1326,7 @@
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="53" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="9">
@@ -1341,8 +1339,8 @@
       <c r="F14" s="10">
         <v>28</v>
       </c>
-      <c r="G14" s="51" t="s">
-        <v>33</v>
+      <c r="G14" s="47" t="s">
+        <v>30</v>
       </c>
       <c r="H14" s="10">
         <v>29</v>
@@ -1355,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N14" s="10">
         <v>2</v>
@@ -1366,50 +1364,50 @@
       </c>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="1:17" s="46" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="40">
+    <row r="15" spans="1:17" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="36">
         <v>12</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="37">
         <v>4</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="47">
+      <c r="E15" s="38"/>
+      <c r="F15" s="43">
         <v>5</v>
       </c>
-      <c r="G15" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="49">
+      <c r="G15" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="45">
         <v>6</v>
       </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="41">
+      <c r="I15" s="39"/>
+      <c r="J15" s="37">
         <v>7</v>
       </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="41">
+      <c r="K15" s="40"/>
+      <c r="L15" s="37">
         <v>8</v>
       </c>
-      <c r="M15" s="45" t="s">
+      <c r="M15" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="37">
+        <v>9</v>
+      </c>
+      <c r="O15" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="N15" s="41">
-        <v>9</v>
-      </c>
-      <c r="O15" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="P15" s="41">
+      <c r="P15" s="37">
         <v>10</v>
       </c>
-      <c r="Q15" s="42"/>
+      <c r="Q15" s="38"/>
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="36"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="9">
         <v>13</v>
       </c>
@@ -1417,11 +1415,11 @@
         <v>11</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="48">
+      <c r="F16" s="44">
         <v>12</v>
       </c>
-      <c r="G16" s="54"/>
-      <c r="H16" s="50">
+      <c r="G16" s="50"/>
+      <c r="H16" s="46">
         <v>13</v>
       </c>
       <c r="J16" s="10">
@@ -1442,7 +1440,7 @@
     </row>
     <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="36"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="9">
         <v>14</v>
       </c>
@@ -1453,7 +1451,7 @@
       <c r="F17" s="10">
         <v>19</v>
       </c>
-      <c r="G17" s="52"/>
+      <c r="G17" s="48"/>
       <c r="H17" s="10">
         <v>20</v>
       </c>
@@ -1477,7 +1475,7 @@
     </row>
     <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="36"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="9">
         <v>15</v>
       </c>
@@ -1512,7 +1510,7 @@
     </row>
     <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="53" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="9">
@@ -1549,7 +1547,7 @@
     </row>
     <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="36"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="9">
         <v>17</v>
       </c>
@@ -1584,7 +1582,7 @@
     </row>
     <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="36"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="9">
         <v>18</v>
       </c>
@@ -1621,7 +1619,7 @@
     </row>
     <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="36"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="9">
         <v>19</v>
       </c>
@@ -6241,6 +6239,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="F3:G3"/>
@@ -6248,11 +6251,6 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>